<commit_message>
Startdate and enddate added to code list
</commit_message>
<xml_diff>
--- a/test_files/Code_list_with_30_Codes.xlsx
+++ b/test_files/Code_list_with_30_Codes.xlsx
@@ -17,96 +17,99 @@
     <t>CODEVALUE</t>
   </si>
   <si>
+    <t>ORGANIZATION</t>
+  </si>
+  <si>
+    <t>INFORMATIONDOMAIN</t>
+  </si>
+  <si>
+    <t>VERSION</t>
+  </si>
+  <si>
+    <t>STATUS</t>
+  </si>
+  <si>
+    <t>PREFLABEL_FI</t>
+  </si>
+  <si>
+    <t>PREFLABEL_SV</t>
+  </si>
+  <si>
+    <t>PREFLABEL_EN</t>
+  </si>
+  <si>
+    <t>DEFINITION_FI</t>
+  </si>
+  <si>
+    <t>DEFINITION_SV</t>
+  </si>
+  <si>
+    <t>DEFINITION_EN</t>
+  </si>
+  <si>
+    <t>DESCRIPTION_FI</t>
+  </si>
+  <si>
+    <t>DESCRIPTION_SV</t>
+  </si>
+  <si>
+    <t>DESCRIPTION_EN</t>
+  </si>
+  <si>
+    <t>CHANGENOTE_FI</t>
+  </si>
+  <si>
+    <t>CHANGENOTE_SV</t>
+  </si>
+  <si>
+    <t>CHANGENOTE_EN</t>
+  </si>
+  <si>
+    <t>STARTDATE</t>
+  </si>
+  <si>
+    <t>ENDDATE</t>
+  </si>
+  <si>
+    <t>SOURCE</t>
+  </si>
+  <si>
     <t>ID</t>
   </si>
   <si>
-    <t>STATUS</t>
+    <t>LEGALBASE</t>
+  </si>
+  <si>
+    <t>GOVERNANCEPOLICY</t>
+  </si>
+  <si>
+    <t>LICENSE</t>
   </si>
   <si>
     <t>HIERARCHYLEVEL</t>
   </si>
   <si>
-    <t>PREFLABEL_FI</t>
-  </si>
-  <si>
-    <t>PREFLABEL_SV</t>
-  </si>
-  <si>
-    <t>PREFLABEL_EN</t>
-  </si>
-  <si>
-    <t>DESCRIPTION_FI</t>
-  </si>
-  <si>
-    <t>ORGANIZATION</t>
-  </si>
-  <si>
-    <t>DESCRIPTION_SV</t>
-  </si>
-  <si>
-    <t>DESCRIPTION_EN</t>
-  </si>
-  <si>
-    <t>INFORMATIONDOMAIN</t>
+    <t>74a41211-8c99-4835-a519-7a61612b1098</t>
+  </si>
+  <si>
+    <t>P1</t>
   </si>
   <si>
     <t>SHORTNAME</t>
   </si>
   <si>
-    <t>STARTDATE</t>
-  </si>
-  <si>
-    <t>ENDDATE</t>
-  </si>
-  <si>
     <t>testcode28</t>
   </si>
   <si>
-    <t>VERSION</t>
-  </si>
-  <si>
-    <t>DEFINITION_FI</t>
-  </si>
-  <si>
-    <t>DEFINITION_SV</t>
-  </si>
-  <si>
-    <t>DEFINITION_EN</t>
-  </si>
-  <si>
-    <t>CHANGENOTE_FI</t>
-  </si>
-  <si>
-    <t>CHANGENOTE_SV</t>
-  </si>
-  <si>
-    <t>CHANGENOTE_EN</t>
-  </si>
-  <si>
-    <t>SOURCE</t>
-  </si>
-  <si>
-    <t>LEGALBASE</t>
-  </si>
-  <si>
-    <t>GOVERNANCEPOLICY</t>
-  </si>
-  <si>
-    <t>LICENSE</t>
-  </si>
-  <si>
-    <t>74a41211-8c99-4835-a519-7a61612b1098</t>
-  </si>
-  <si>
-    <t>P1</t>
-  </si>
-  <si>
     <t>DRAFT</t>
   </si>
   <si>
     <t>Testcode 28</t>
   </si>
   <si>
+    <t>Koodisto600</t>
+  </si>
+  <si>
     <t>testcode29</t>
   </si>
   <si>
@@ -165,9 +168,6 @@
   </si>
   <si>
     <t>Testcode 38</t>
-  </si>
-  <si>
-    <t>Koodisto600</t>
   </si>
   <si>
     <t>testcode39</t>
@@ -288,6 +288,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+  </numFmts>
   <fonts count="3">
     <font>
       <sz val="10.0"/>
@@ -329,17 +332,17 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -368,7 +371,8 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="2" width="35.86"/>
-    <col customWidth="1" min="3" max="5" width="14.43"/>
+    <col customWidth="1" min="3" max="3" width="25.0"/>
+    <col customWidth="1" min="4" max="5" width="14.43"/>
     <col customWidth="1" min="6" max="6" width="22.29"/>
     <col customWidth="1" min="7" max="7" width="14.43"/>
   </cols>
@@ -378,70 +382,70 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="P1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="T1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
@@ -449,19 +453,19 @@
         <v>600.0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="5">
+        <v>25</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="4">
         <v>1.0</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>51</v>
+      <c r="E2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -474,8 +478,12 @@
       <c r="O2" s="1"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="1"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
+      <c r="R2" s="5">
+        <v>43101.0</v>
+      </c>
+      <c r="S2" s="5">
+        <v>43466.0</v>
+      </c>
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
       <c r="V2" s="3"/>
@@ -1502,45 +1510,45 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="1" t="s">
@@ -1561,7 +1569,7 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
@@ -1569,7 +1577,7 @@
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -1582,101 +1590,101 @@
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
Code list name changed in test case 200 and 203
</commit_message>
<xml_diff>
--- a/test_files/Code_list_with_30_Codes.xlsx
+++ b/test_files/Code_list_with_30_Codes.xlsx
@@ -1,13 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21412"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A057DEFE-2F59-4EBE-9191-1635F74230E4}" xr6:coauthVersionLast="42" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="CodeSchemes" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="Codes" sheetId="2" r:id="rId4"/>
+    <sheet name="CodeSchemes" sheetId="1" r:id="rId1"/>
+    <sheet name="Codes" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -74,40 +86,40 @@
     <t>SOURCE</t>
   </si>
   <si>
+    <t>LEGALBASE</t>
+  </si>
+  <si>
+    <t>GOVERNANCEPOLICY</t>
+  </si>
+  <si>
+    <t>LICENSE</t>
+  </si>
+  <si>
+    <t>74a41211-8c99-4835-a519-7a61612b1098</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>DRAFT</t>
+  </si>
+  <si>
+    <t>koodisto6000</t>
+  </si>
+  <si>
     <t>ID</t>
   </si>
   <si>
-    <t>LEGALBASE</t>
-  </si>
-  <si>
-    <t>GOVERNANCEPOLICY</t>
-  </si>
-  <si>
-    <t>LICENSE</t>
-  </si>
-  <si>
     <t>HIERARCHYLEVEL</t>
   </si>
   <si>
-    <t>74a41211-8c99-4835-a519-7a61612b1098</t>
-  </si>
-  <si>
-    <t>P1</t>
-  </si>
-  <si>
     <t>SHORTNAME</t>
   </si>
   <si>
     <t>testcode28</t>
   </si>
   <si>
-    <t>DRAFT</t>
-  </si>
-  <si>
     <t>Testcode 28</t>
-  </si>
-  <si>
-    <t>Koodisto600</t>
   </si>
   <si>
     <t>testcode29</t>
@@ -287,21 +299,23 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="3">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -310,7 +324,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -320,64 +334,361 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:W1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="35.86"/>
-    <col customWidth="1" min="3" max="3" width="25.0"/>
-    <col customWidth="1" min="4" max="5" width="14.43"/>
-    <col customWidth="1" min="6" max="6" width="22.29"/>
-    <col customWidth="1" min="7" max="7" width="14.43"/>
+    <col min="1" max="2" width="35.85546875" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:23" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -439,33 +750,33 @@
         <v>19</v>
       </c>
       <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="W1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:23" ht="15.75" customHeight="1">
+      <c r="A2" s="1">
+        <v>6000</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="1">
-        <v>600.0</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="D2" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -479,30 +790,30 @@
       <c r="P2" s="3"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="5">
-        <v>43101.0</v>
+        <v>43101</v>
       </c>
       <c r="S2" s="5">
-        <v>43466.0</v>
+        <v>43466</v>
       </c>
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
     </row>
-    <row r="3" ht="15.75" customHeight="1"/>
-    <row r="4" ht="15.75" customHeight="1"/>
-    <row r="5" ht="15.75" customHeight="1"/>
-    <row r="6" ht="15.75" customHeight="1"/>
-    <row r="7" ht="15.75" customHeight="1"/>
-    <row r="8" ht="15.75" customHeight="1"/>
-    <row r="9" ht="15.75" customHeight="1"/>
-    <row r="10" ht="15.75" customHeight="1"/>
-    <row r="11" ht="15.75" customHeight="1"/>
-    <row r="12" ht="15.75" customHeight="1"/>
-    <row r="13" ht="15.75" customHeight="1"/>
-    <row r="14" ht="15.75" customHeight="1"/>
-    <row r="15" ht="15.75" customHeight="1"/>
-    <row r="16" ht="15.75" customHeight="1"/>
+    <row r="3" spans="1:23" ht="15.75" customHeight="1"/>
+    <row r="4" spans="1:23" ht="15.75" customHeight="1"/>
+    <row r="5" spans="1:23" ht="15.75" customHeight="1"/>
+    <row r="6" spans="1:23" ht="15.75" customHeight="1"/>
+    <row r="7" spans="1:23" ht="15.75" customHeight="1"/>
+    <row r="8" spans="1:23" ht="15.75" customHeight="1"/>
+    <row r="9" spans="1:23" ht="15.75" customHeight="1"/>
+    <row r="10" spans="1:23" ht="15.75" customHeight="1"/>
+    <row r="11" spans="1:23" ht="15.75" customHeight="1"/>
+    <row r="12" spans="1:23" ht="15.75" customHeight="1"/>
+    <row r="13" spans="1:23" ht="15.75" customHeight="1"/>
+    <row r="14" spans="1:23" ht="15.75" customHeight="1"/>
+    <row r="15" spans="1:23" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:23" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -1488,35 +1799,36 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:M1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="6" width="14.43"/>
+    <col min="1" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:13" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>5</v>
@@ -1537,7 +1849,7 @@
         <v>13</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>17</v>
@@ -1546,17 +1858,17 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:13" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -1567,13 +1879,13 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:13" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
@@ -1588,315 +1900,315 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:13" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
+    <row r="5" spans="1:13" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:13" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:13" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
+    <row r="8" spans="1:13" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" ht="15.75" customHeight="1">
+    <row r="9" spans="1:13" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" ht="15.75" customHeight="1">
+    <row r="10" spans="1:13" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="11" ht="15.75" customHeight="1">
+    <row r="11" spans="1:13" ht="15.75" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="12" ht="15.75" customHeight="1">
+    <row r="12" spans="1:13" ht="15.75" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
+    <row r="13" spans="1:13" ht="15.75" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="14" ht="15.75" customHeight="1">
+    <row r="14" spans="1:13" ht="15.75" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="15" ht="15.75" customHeight="1">
+    <row r="15" spans="1:13" ht="15.75" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="16" ht="15.75" customHeight="1">
+    <row r="16" spans="1:13" ht="15.75" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="17" ht="15.75" customHeight="1">
+    <row r="17" spans="1:5" ht="15.75" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>60</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="18" ht="15.75" customHeight="1">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="19" ht="15.75" customHeight="1">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>64</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="20" ht="15.75" customHeight="1">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
+    <row r="21" spans="1:5" ht="15.75" customHeight="1">
       <c r="A21" s="1" t="s">
         <v>68</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
+    <row r="22" spans="1:5" ht="15.75" customHeight="1">
       <c r="A22" s="1" t="s">
         <v>70</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
+    <row r="23" spans="1:5" ht="15.75" customHeight="1">
       <c r="A23" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
+    <row r="24" spans="1:5" ht="15.75" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>74</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="25" ht="15.75" customHeight="1">
+    <row r="25" spans="1:5" ht="15.75" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>76</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="26" ht="15.75" customHeight="1">
+    <row r="26" spans="1:5" ht="15.75" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>78</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="27" ht="15.75" customHeight="1">
+    <row r="27" spans="1:5" ht="15.75" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="28" ht="15.75" customHeight="1">
+    <row r="28" spans="1:5" ht="15.75" customHeight="1">
       <c r="A28" s="1" t="s">
         <v>82</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="29" ht="15.75" customHeight="1">
+    <row r="29" spans="1:5" ht="15.75" customHeight="1">
       <c r="A29" s="1" t="s">
         <v>84</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
+    <row r="30" spans="1:5" ht="15.75" customHeight="1">
       <c r="A30" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
+    <row r="31" spans="1:5" ht="15.75" customHeight="1">
       <c r="A31" s="1" t="s">
         <v>88</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="32" spans="1:5" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -2866,6 +3178,6 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
 </worksheet>
 </file>
</xml_diff>